<commit_message>
Updated term project requirements and rubric
</commit_message>
<xml_diff>
--- a/TermProject/TermProjectRubric_CS295N.xlsx
+++ b/TermProject/TermProjectRubric_CS295N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F214BF7-D654-5246-954C-F5DD5BCF3181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDB758C-CF76-804D-9FF8-2360C09FE8D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23520" windowHeight="14740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23520" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Overall functionality</t>
   </si>
   <si>
-    <t>Running on SmarterASP.NET</t>
-  </si>
-  <si>
     <t>Unit tests passing</t>
   </si>
   <si>
-    <t>Seed Data</t>
-  </si>
-  <si>
     <t>Site navigation</t>
   </si>
   <si>
@@ -69,6 +63,15 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>Running on Azure</t>
+  </si>
+  <si>
+    <t>Interactive feature</t>
+  </si>
+  <si>
+    <t>CS295N Term Project Rubric</t>
   </si>
 </sst>
 </file>
@@ -982,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -995,284 +998,274 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="6"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="A4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="F5" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>20</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
       <c r="B10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>50</v>
+      <c r="A12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4">
+        <f>SUM(B3:B12)</f>
+        <v>100</v>
+      </c>
+      <c r="C13" s="4">
+        <f>SUM(C3:C12)</f>
+        <v>100</v>
+      </c>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="12">
-        <v>40</v>
-      </c>
-      <c r="C14" s="12">
-        <v>40</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4">
-        <f>SUM(B5:B14)</f>
-        <v>340</v>
-      </c>
-      <c r="C15" s="4">
-        <f>SUM(C5:C14)</f>
-        <v>340</v>
-      </c>
-      <c r="D15" s="12"/>
+      <c r="A15" s="8"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="8"/>
+      <c r="A17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6">
+      <c r="A18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6"/>
+      <c r="A20" s="1"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="1"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6">
+      <c r="A24" s="4"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="4"/>
-      <c r="F26" s="6"/>
-    </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="6"/>
+      <c r="A27" s="4"/>
       <c r="F27" s="6"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="4"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="31" spans="1:6">
-      <c r="F31" s="6"/>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="4"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="34" spans="1:6">
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6">
+    <row r="33" spans="1:3">
+      <c r="A33" s="12"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="12"/>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="12"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="12"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="7"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="8"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="6"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:6">
+    <row r="36" spans="1:3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="6"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="9"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="4"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="55" spans="1:3" s="4" customFormat="1"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="53" spans="1:3" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1282,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C8BAC4-7C35-B64C-9C0F-AC9B3324E891}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1317,95 +1310,95 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="F5" s="6"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
-        <v>13</v>
+      <c r="A8" t="s">
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1413,10 +1406,10 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -1425,11 +1418,12 @@
         <v>7</v>
       </c>
       <c r="B14" s="12">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C14" s="12">
-        <v>40</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E14"/>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
@@ -1438,11 +1432,11 @@
       </c>
       <c r="B15" s="4">
         <f>SUM(B5:B14)</f>
-        <v>340</v>
+        <v>100</v>
       </c>
       <c r="C15" s="4">
         <f>SUM(C5:C14)</f>
-        <v>340</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
Term project requirement updates
</commit_message>
<xml_diff>
--- a/TermProject/TermProjectRubric_CS295N.xlsx
+++ b/TermProject/TermProjectRubric_CS295N.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS295N-CourseMaterials/TermProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS295N-CourseMaterials\TermProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDB758C-CF76-804D-9FF8-2360C09FE8D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0895924E-CD73-4A8A-ACBF-439A4F5D5959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23520" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4416" yWindow="2004" windowWidth="15360" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Student Points" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>-----------------------------------</t>
   </si>
@@ -68,10 +81,22 @@
     <t>Running on Azure</t>
   </si>
   <si>
-    <t>Interactive feature</t>
-  </si>
-  <si>
     <t>CS295N Term Project Rubric</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (7 * 3)</t>
+  </si>
+  <si>
+    <t>(4 * 6)</t>
+  </si>
+  <si>
+    <t>Interactive logical processing feature</t>
   </si>
 </sst>
 </file>
@@ -609,7 +634,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -628,8 +653,10 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,18 +1014,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1006,42 +1034,37 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.399999999999999">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -1050,10 +1073,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1061,68 +1081,50 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12">
-        <v>10</v>
+      <c r="B12">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1131,13 +1133,9 @@
       </c>
       <c r="B13" s="4">
         <f>SUM(B3:B12)</f>
-        <v>100</v>
-      </c>
-      <c r="C13" s="4">
-        <f>SUM(C3:C12)</f>
-        <v>100</v>
-      </c>
-      <c r="D13" s="12"/>
+        <v>340</v>
+      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="3"/>
@@ -1202,15 +1200,6 @@
     </row>
     <row r="32" spans="1:6">
       <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="12"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="12"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="12"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="7"/>
@@ -1275,16 +1264,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C8BAC4-7C35-B64C-9C0F-AC9B3324E891}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.296875" customWidth="1"/>
+    <col min="2" max="2" width="7.8984375" customWidth="1"/>
+    <col min="3" max="3" width="5.8984375" customWidth="1"/>
+    <col min="4" max="4" width="1.8984375" customWidth="1"/>
+    <col min="5" max="5" width="7.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1288,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1313,21 +1306,21 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6"/>
     </row>
@@ -1336,10 +1329,10 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1347,10 +1340,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F8" s="6"/>
     </row>
@@ -1359,72 +1352,77 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
       </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="12" t="s">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="12" t="s">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" s="12" customFormat="1">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="12">
-        <v>10</v>
-      </c>
-      <c r="C14" s="12">
-        <v>10</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14" s="13"/>
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>33</v>
+      </c>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1">
       <c r="A15" s="4" t="s">
@@ -1432,11 +1430,18 @@
       </c>
       <c r="B15" s="4">
         <f>SUM(B5:B14)</f>
-        <v>100</v>
+        <v>340</v>
       </c>
       <c r="C15" s="4">
         <f>SUM(C5:C14)</f>
-        <v>100</v>
+        <v>248</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="14">
+        <f>C15/B15</f>
+        <v>0.72941176470588232</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1495,15 +1500,10 @@
     <row r="33" spans="1:6">
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12"/>
-    </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="12"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="12"/>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6">
@@ -1539,5 +1539,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>